<commit_message>
sule to shwedagon finish
</commit_message>
<xml_diff>
--- a/haversine/distance_csv/dist.xlsx
+++ b/haversine/distance_csv/dist.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Sule</t>
+    <t>a</t>
   </si>
   <si>
-    <t>Sule Myodaw Hall</t>
+    <t>b</t>
   </si>
   <si>
-    <t>Yoke Shin Yone</t>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -854,7 +854,7 @@
   <dimension ref="A3:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>